<commit_message>
War with the combined cells.
</commit_message>
<xml_diff>
--- a/Шаблон_CalibrationIRT59xx.xlsx
+++ b/Шаблон_CalibrationIRT59xx.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="62">
   <si>
     <t>ПРОТОКОЛ КАЛИБРОВКИ №</t>
   </si>
@@ -122,9 +122,6 @@
     <t xml:space="preserve">абсолютное значение, </t>
   </si>
   <si>
-    <t xml:space="preserve">24 </t>
-  </si>
-  <si>
     <t>Заключение по результатам калибровки всех каналов</t>
   </si>
   <si>
@@ -149,9 +146,6 @@
     <t>Унифицированный выходной сигнал постоянного тока</t>
   </si>
   <si>
-    <t>напряжение, В</t>
-  </si>
-  <si>
     <t>Значение входного сигнала, %</t>
   </si>
   <si>
@@ -164,9 +158,6 @@
     <t>допускаемая основная приведенная погрешность, %</t>
   </si>
   <si>
-    <t>ток, мА</t>
-  </si>
-  <si>
     <t>Тип, модель ИП:</t>
   </si>
   <si>
@@ -207,6 +198,18 @@
   </si>
   <si>
     <t>Модель:</t>
+  </si>
+  <si>
+    <t>ток</t>
+  </si>
+  <si>
+    <t>—</t>
+  </si>
+  <si>
+    <t>24В</t>
+  </si>
+  <si>
+    <t>напряжение</t>
   </si>
 </sst>
 </file>
@@ -1642,10 +1645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R100"/>
+  <dimension ref="A1:R98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="G86" sqref="G86:H86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1688,7 +1691,7 @@
     </row>
     <row r="3" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B3" s="46"/>
       <c r="C3" s="46"/>
@@ -1702,7 +1705,7 @@
     </row>
     <row r="4" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -1736,13 +1739,13 @@
     </row>
     <row r="8" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="150" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>3</v>
       </c>
       <c r="H8" s="151" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="K8" s="15"/>
       <c r="P8" s="13"/>
@@ -1750,7 +1753,7 @@
     </row>
     <row r="9" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="150" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>4</v>
@@ -1758,7 +1761,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="150" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="P9" s="9"/>
       <c r="Q9" s="2"/>
@@ -1766,10 +1769,10 @@
     </row>
     <row r="10" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="152" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H10" s="151" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="P10" s="10"/>
       <c r="Q10" s="10"/>
@@ -1803,35 +1806,35 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="150" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B14" s="7"/>
       <c r="E14" s="17" t="s">
         <v>7</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I14" s="13"/>
       <c r="K14" s="15"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="152" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B15" s="23"/>
       <c r="E15" s="17">
         <v>2</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I15" s="13"/>
       <c r="K15" s="15"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="152" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B16" s="23"/>
       <c r="E16" s="17"/>
@@ -1841,7 +1844,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="152" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B17" s="23"/>
       <c r="E17" s="17"/>
@@ -1851,7 +1854,7 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="152" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B18" s="23"/>
       <c r="E18" s="17"/>
@@ -2025,7 +2028,7 @@
     </row>
     <row r="29" spans="1:15" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="45" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="6"/>
@@ -2141,7 +2144,7 @@
     </row>
     <row r="35" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="35" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B35" s="36"/>
       <c r="C35" s="36"/>
@@ -2204,7 +2207,7 @@
       </c>
       <c r="B39" s="81"/>
       <c r="C39" s="94" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D39" s="94"/>
       <c r="E39" s="77"/>
@@ -2349,7 +2352,7 @@
     </row>
     <row r="48" spans="1:15" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="12"/>
@@ -2402,116 +2405,111 @@
       <c r="N50" s="93"/>
     </row>
     <row r="51" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="B51" s="27"/>
-      <c r="C51" s="27"/>
-      <c r="D51" s="28"/>
-      <c r="E51" s="28"/>
-      <c r="F51" s="28"/>
-      <c r="G51" s="29"/>
-      <c r="H51" s="63" t="s">
-        <v>41</v>
-      </c>
-      <c r="I51" s="63"/>
-      <c r="J51" s="63"/>
-      <c r="K51" s="64" t="s">
-        <v>32</v>
-      </c>
-      <c r="L51" s="63"/>
-      <c r="M51" s="63"/>
-      <c r="N51" s="66"/>
-    </row>
-    <row r="52" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="30" t="s">
+      <c r="A51" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B52" s="31"/>
-      <c r="C52" s="31"/>
-      <c r="D52" s="32"/>
-      <c r="E52" s="32"/>
-      <c r="F52" s="32"/>
-      <c r="G52" s="44"/>
-      <c r="H52" s="67" t="s">
-        <v>19</v>
-      </c>
-      <c r="I52" s="67"/>
-      <c r="J52" s="67"/>
-      <c r="K52" s="68" t="s">
-        <v>32</v>
-      </c>
-      <c r="L52" s="67"/>
-      <c r="M52" s="67"/>
-      <c r="N52" s="69"/>
-    </row>
-    <row r="53" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="B53" s="36"/>
-      <c r="C53" s="36"/>
-      <c r="D53" s="36"/>
-      <c r="E53" s="36"/>
-      <c r="F53" s="36"/>
-      <c r="G53" s="37"/>
-      <c r="H53" s="70"/>
-      <c r="I53" s="71"/>
-      <c r="J53" s="71"/>
-      <c r="K53" s="71"/>
-      <c r="L53" s="71"/>
-      <c r="M53" s="71"/>
-      <c r="N53" s="72"/>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C54" s="38"/>
-      <c r="D54" s="38"/>
-      <c r="E54" s="38"/>
-      <c r="F54" s="38"/>
-      <c r="G54" s="38"/>
-    </row>
-    <row r="55" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+      <c r="B51" s="31"/>
+      <c r="C51" s="31"/>
+      <c r="D51" s="32"/>
+      <c r="E51" s="32"/>
+      <c r="F51" s="32"/>
+      <c r="G51" s="44"/>
+      <c r="H51" s="67" t="s">
+        <v>61</v>
+      </c>
+      <c r="I51" s="67"/>
+      <c r="J51" s="67"/>
+      <c r="K51" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="L51" s="67"/>
+      <c r="M51" s="67"/>
+      <c r="N51" s="69"/>
+    </row>
+    <row r="52" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="B52" s="36"/>
+      <c r="C52" s="36"/>
+      <c r="D52" s="36"/>
+      <c r="E52" s="36"/>
+      <c r="F52" s="36"/>
+      <c r="G52" s="37"/>
+      <c r="H52" s="70"/>
+      <c r="I52" s="71"/>
+      <c r="J52" s="71"/>
+      <c r="K52" s="71"/>
+      <c r="L52" s="71"/>
+      <c r="M52" s="71"/>
+      <c r="N52" s="72"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C53" s="38"/>
+      <c r="D53" s="38"/>
+      <c r="E53" s="38"/>
+      <c r="F53" s="38"/>
+      <c r="G53" s="38"/>
+    </row>
+    <row r="54" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>23</v>
       </c>
     </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A55" s="73" t="s">
+        <v>24</v>
+      </c>
+      <c r="B55" s="74"/>
+      <c r="C55" s="74"/>
+      <c r="D55" s="74"/>
+      <c r="E55" s="75" t="s">
+        <v>25</v>
+      </c>
+      <c r="F55" s="76"/>
+      <c r="G55" s="75" t="s">
+        <v>26</v>
+      </c>
+      <c r="H55" s="76"/>
+      <c r="I55" s="74" t="s">
+        <v>27</v>
+      </c>
+      <c r="J55" s="74"/>
+      <c r="K55" s="74" t="s">
+        <v>28</v>
+      </c>
+      <c r="L55" s="74"/>
+      <c r="M55" s="74" t="s">
+        <v>29</v>
+      </c>
+      <c r="N55" s="83"/>
+      <c r="O55" s="39"/>
+    </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A56" s="73" t="s">
-        <v>24</v>
-      </c>
-      <c r="B56" s="74"/>
-      <c r="C56" s="74"/>
-      <c r="D56" s="74"/>
-      <c r="E56" s="75" t="s">
-        <v>25</v>
-      </c>
-      <c r="F56" s="76"/>
-      <c r="G56" s="75" t="s">
-        <v>26</v>
-      </c>
-      <c r="H56" s="76"/>
-      <c r="I56" s="74" t="s">
-        <v>27</v>
-      </c>
-      <c r="J56" s="74"/>
-      <c r="K56" s="74" t="s">
-        <v>28</v>
-      </c>
-      <c r="L56" s="74"/>
-      <c r="M56" s="74" t="s">
-        <v>29</v>
-      </c>
-      <c r="N56" s="83"/>
+      <c r="A56" s="86" t="s">
+        <v>40</v>
+      </c>
+      <c r="B56" s="81"/>
+      <c r="C56" s="94" t="s">
+        <v>42</v>
+      </c>
+      <c r="D56" s="94"/>
+      <c r="E56" s="77"/>
+      <c r="F56" s="78"/>
+      <c r="G56" s="77"/>
+      <c r="H56" s="78"/>
+      <c r="I56" s="81"/>
+      <c r="J56" s="81"/>
+      <c r="K56" s="81"/>
+      <c r="L56" s="81"/>
+      <c r="M56" s="81"/>
+      <c r="N56" s="84"/>
       <c r="O56" s="39"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A57" s="86" t="s">
-        <v>42</v>
-      </c>
+      <c r="A57" s="86"/>
       <c r="B57" s="81"/>
-      <c r="C57" s="94" t="s">
-        <v>44</v>
-      </c>
+      <c r="C57" s="94"/>
       <c r="D57" s="94"/>
       <c r="E57" s="77"/>
       <c r="F57" s="78"/>
@@ -2525,497 +2523,498 @@
       <c r="N57" s="84"/>
       <c r="O57" s="39"/>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A58" s="86"/>
-      <c r="B58" s="81"/>
-      <c r="C58" s="94"/>
-      <c r="D58" s="94"/>
-      <c r="E58" s="77"/>
-      <c r="F58" s="78"/>
-      <c r="G58" s="77"/>
-      <c r="H58" s="78"/>
-      <c r="I58" s="81"/>
-      <c r="J58" s="81"/>
-      <c r="K58" s="81"/>
-      <c r="L58" s="81"/>
-      <c r="M58" s="81"/>
-      <c r="N58" s="84"/>
+    <row r="58" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="87"/>
+      <c r="B58" s="82"/>
+      <c r="C58" s="95"/>
+      <c r="D58" s="95"/>
+      <c r="E58" s="79"/>
+      <c r="F58" s="80"/>
+      <c r="G58" s="79"/>
+      <c r="H58" s="80"/>
+      <c r="I58" s="82"/>
+      <c r="J58" s="82"/>
+      <c r="K58" s="82"/>
+      <c r="L58" s="82"/>
+      <c r="M58" s="82"/>
+      <c r="N58" s="85"/>
       <c r="O58" s="39"/>
     </row>
-    <row r="59" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="87"/>
-      <c r="B59" s="82"/>
-      <c r="C59" s="95"/>
-      <c r="D59" s="95"/>
-      <c r="E59" s="79"/>
-      <c r="F59" s="80"/>
-      <c r="G59" s="79"/>
-      <c r="H59" s="80"/>
-      <c r="I59" s="82"/>
-      <c r="J59" s="82"/>
-      <c r="K59" s="82"/>
-      <c r="L59" s="82"/>
-      <c r="M59" s="82"/>
-      <c r="N59" s="85"/>
-      <c r="O59" s="39"/>
-    </row>
-    <row r="60" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="55">
+    <row r="59" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="55">
         <v>100</v>
       </c>
-      <c r="B60" s="56"/>
-      <c r="C60" s="57"/>
-      <c r="D60" s="57"/>
-      <c r="E60" s="58"/>
-      <c r="F60" s="59"/>
-      <c r="G60" s="58"/>
-      <c r="H60" s="59"/>
-      <c r="I60" s="60"/>
-      <c r="J60" s="60"/>
-      <c r="K60" s="60"/>
-      <c r="L60" s="60"/>
-      <c r="M60" s="61"/>
-      <c r="N60" s="62"/>
-    </row>
-    <row r="62" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="10" t="s">
+      <c r="B59" s="56"/>
+      <c r="C59" s="57"/>
+      <c r="D59" s="57"/>
+      <c r="E59" s="58" t="s">
+        <v>59</v>
+      </c>
+      <c r="F59" s="59"/>
+      <c r="G59" s="58"/>
+      <c r="H59" s="59"/>
+      <c r="I59" s="60"/>
+      <c r="J59" s="60"/>
+      <c r="K59" s="60"/>
+      <c r="L59" s="60"/>
+      <c r="M59" s="61"/>
+      <c r="N59" s="62"/>
+    </row>
+    <row r="61" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B61" s="2"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6"/>
+      <c r="H61" s="6"/>
+      <c r="I61" s="6"/>
+      <c r="J61" s="6"/>
+      <c r="K61" s="6"/>
+      <c r="L61" s="6"/>
+      <c r="M61" s="6"/>
+      <c r="N61" s="6"/>
+    </row>
+    <row r="62" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="88"/>
+      <c r="B62" s="89"/>
+      <c r="C62" s="89"/>
+      <c r="D62" s="89"/>
+      <c r="E62" s="89"/>
+      <c r="F62" s="89"/>
+      <c r="G62" s="90"/>
+      <c r="H62" s="89" t="s">
+        <v>14</v>
+      </c>
+      <c r="I62" s="89"/>
+      <c r="J62" s="89"/>
+      <c r="K62" s="96" t="s">
+        <v>15</v>
+      </c>
+      <c r="L62" s="89"/>
+      <c r="M62" s="89"/>
+      <c r="N62" s="90"/>
+    </row>
+    <row r="63" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="91"/>
+      <c r="B63" s="92"/>
+      <c r="C63" s="92"/>
+      <c r="D63" s="92"/>
+      <c r="E63" s="92"/>
+      <c r="F63" s="92"/>
+      <c r="G63" s="93"/>
+      <c r="H63" s="92"/>
+      <c r="I63" s="92"/>
+      <c r="J63" s="92"/>
+      <c r="K63" s="97"/>
+      <c r="L63" s="92"/>
+      <c r="M63" s="92"/>
+      <c r="N63" s="93"/>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A64" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B64" s="31"/>
+      <c r="C64" s="31"/>
+      <c r="D64" s="32"/>
+      <c r="E64" s="32"/>
+      <c r="F64" s="32"/>
+      <c r="G64" s="44"/>
+      <c r="H64" s="67" t="s">
+        <v>61</v>
+      </c>
+      <c r="I64" s="67"/>
+      <c r="J64" s="67"/>
+      <c r="K64" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="L64" s="67"/>
+      <c r="M64" s="67"/>
+      <c r="N64" s="69"/>
+    </row>
+    <row r="65" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="B65" s="36"/>
+      <c r="C65" s="36"/>
+      <c r="D65" s="36"/>
+      <c r="E65" s="36"/>
+      <c r="F65" s="36"/>
+      <c r="G65" s="37"/>
+      <c r="H65" s="70"/>
+      <c r="I65" s="71"/>
+      <c r="J65" s="71"/>
+      <c r="K65" s="71"/>
+      <c r="L65" s="71"/>
+      <c r="M65" s="71"/>
+      <c r="N65" s="72"/>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C66" s="38"/>
+      <c r="D66" s="38"/>
+      <c r="E66" s="38"/>
+      <c r="F66" s="38"/>
+      <c r="G66" s="38"/>
+    </row>
+    <row r="67" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A68" s="73" t="s">
+        <v>24</v>
+      </c>
+      <c r="B68" s="74"/>
+      <c r="C68" s="74"/>
+      <c r="D68" s="74"/>
+      <c r="E68" s="75" t="s">
+        <v>25</v>
+      </c>
+      <c r="F68" s="76"/>
+      <c r="G68" s="75" t="s">
+        <v>26</v>
+      </c>
+      <c r="H68" s="76"/>
+      <c r="I68" s="74" t="s">
+        <v>27</v>
+      </c>
+      <c r="J68" s="74"/>
+      <c r="K68" s="74" t="s">
+        <v>28</v>
+      </c>
+      <c r="L68" s="74"/>
+      <c r="M68" s="74" t="s">
+        <v>29</v>
+      </c>
+      <c r="N68" s="83"/>
+      <c r="O68" s="39"/>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A69" s="86" t="s">
+        <v>30</v>
+      </c>
+      <c r="B69" s="81"/>
+      <c r="C69" s="94" t="s">
+        <v>31</v>
+      </c>
+      <c r="D69" s="94"/>
+      <c r="E69" s="77"/>
+      <c r="F69" s="78"/>
+      <c r="G69" s="77"/>
+      <c r="H69" s="78"/>
+      <c r="I69" s="81"/>
+      <c r="J69" s="81"/>
+      <c r="K69" s="81"/>
+      <c r="L69" s="81"/>
+      <c r="M69" s="81"/>
+      <c r="N69" s="84"/>
+      <c r="O69" s="39"/>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A70" s="86"/>
+      <c r="B70" s="81"/>
+      <c r="C70" s="94"/>
+      <c r="D70" s="94"/>
+      <c r="E70" s="77"/>
+      <c r="F70" s="78"/>
+      <c r="G70" s="77"/>
+      <c r="H70" s="78"/>
+      <c r="I70" s="81"/>
+      <c r="J70" s="81"/>
+      <c r="K70" s="81"/>
+      <c r="L70" s="81"/>
+      <c r="M70" s="81"/>
+      <c r="N70" s="84"/>
+      <c r="O70" s="39"/>
+    </row>
+    <row r="71" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="87"/>
+      <c r="B71" s="82"/>
+      <c r="C71" s="95"/>
+      <c r="D71" s="95"/>
+      <c r="E71" s="79"/>
+      <c r="F71" s="80"/>
+      <c r="G71" s="79"/>
+      <c r="H71" s="80"/>
+      <c r="I71" s="82"/>
+      <c r="J71" s="82"/>
+      <c r="K71" s="82"/>
+      <c r="L71" s="82"/>
+      <c r="M71" s="82"/>
+      <c r="N71" s="85"/>
+      <c r="O71" s="39"/>
+    </row>
+    <row r="72" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="55">
+        <v>100</v>
+      </c>
+      <c r="B72" s="56"/>
+      <c r="C72" s="57"/>
+      <c r="D72" s="57"/>
+      <c r="E72" s="58" t="s">
+        <v>59</v>
+      </c>
+      <c r="F72" s="59"/>
+      <c r="G72" s="58"/>
+      <c r="H72" s="59"/>
+      <c r="I72" s="60"/>
+      <c r="J72" s="60"/>
+      <c r="K72" s="60"/>
+      <c r="L72" s="60"/>
+      <c r="M72" s="61"/>
+      <c r="N72" s="62"/>
+    </row>
+    <row r="74" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="B62" s="2"/>
-      <c r="C62" s="12"/>
-      <c r="D62" s="6"/>
-      <c r="E62" s="6"/>
-      <c r="F62" s="6"/>
-      <c r="G62" s="6"/>
-      <c r="H62" s="6"/>
-      <c r="I62" s="6"/>
-      <c r="J62" s="6"/>
-      <c r="K62" s="6"/>
-      <c r="L62" s="6"/>
-      <c r="M62" s="6"/>
-      <c r="N62" s="6"/>
-    </row>
-    <row r="63" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="88"/>
-      <c r="B63" s="89"/>
-      <c r="C63" s="89"/>
-      <c r="D63" s="89"/>
-      <c r="E63" s="89"/>
-      <c r="F63" s="89"/>
-      <c r="G63" s="90"/>
-      <c r="H63" s="89" t="s">
+      <c r="B74" s="12"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
+      <c r="I74" s="6"/>
+      <c r="J74" s="6"/>
+      <c r="K74" s="6"/>
+      <c r="L74" s="6"/>
+      <c r="M74" s="6"/>
+      <c r="N74" s="6"/>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A75" s="88"/>
+      <c r="B75" s="89"/>
+      <c r="C75" s="89"/>
+      <c r="D75" s="89"/>
+      <c r="E75" s="89"/>
+      <c r="F75" s="89"/>
+      <c r="G75" s="90"/>
+      <c r="H75" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="I63" s="89"/>
-      <c r="J63" s="89"/>
-      <c r="K63" s="96" t="s">
+      <c r="I75" s="89"/>
+      <c r="J75" s="89"/>
+      <c r="K75" s="137" t="s">
         <v>15</v>
       </c>
-      <c r="L63" s="89"/>
-      <c r="M63" s="89"/>
-      <c r="N63" s="90"/>
-    </row>
-    <row r="64" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="91"/>
-      <c r="B64" s="92"/>
-      <c r="C64" s="92"/>
-      <c r="D64" s="92"/>
-      <c r="E64" s="92"/>
-      <c r="F64" s="92"/>
-      <c r="G64" s="93"/>
-      <c r="H64" s="92"/>
-      <c r="I64" s="92"/>
-      <c r="J64" s="92"/>
-      <c r="K64" s="97"/>
-      <c r="L64" s="92"/>
-      <c r="M64" s="92"/>
-      <c r="N64" s="93"/>
-    </row>
-    <row r="65" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="26" t="s">
+      <c r="L75" s="138"/>
+      <c r="M75" s="138"/>
+      <c r="N75" s="139"/>
+    </row>
+    <row r="76" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="91"/>
+      <c r="B76" s="92"/>
+      <c r="C76" s="92"/>
+      <c r="D76" s="92"/>
+      <c r="E76" s="92"/>
+      <c r="F76" s="92"/>
+      <c r="G76" s="93"/>
+      <c r="H76" s="92"/>
+      <c r="I76" s="92"/>
+      <c r="J76" s="92"/>
+      <c r="K76" s="97" t="s">
+        <v>16</v>
+      </c>
+      <c r="L76" s="140"/>
+      <c r="M76" s="97" t="s">
+        <v>17</v>
+      </c>
+      <c r="N76" s="93"/>
+    </row>
+    <row r="77" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B65" s="27"/>
-      <c r="C65" s="27"/>
-      <c r="D65" s="28"/>
-      <c r="E65" s="28"/>
-      <c r="F65" s="28"/>
-      <c r="G65" s="29"/>
-      <c r="H65" s="63" t="s">
-        <v>41</v>
-      </c>
-      <c r="I65" s="63"/>
-      <c r="J65" s="63"/>
-      <c r="K65" s="64">
+      <c r="B77" s="27"/>
+      <c r="C77" s="27"/>
+      <c r="D77" s="28"/>
+      <c r="E77" s="28"/>
+      <c r="F77" s="28"/>
+      <c r="G77" s="29"/>
+      <c r="H77" s="63"/>
+      <c r="I77" s="63"/>
+      <c r="J77" s="63"/>
+      <c r="K77" s="64"/>
+      <c r="L77" s="65"/>
+      <c r="M77" s="64"/>
+      <c r="N77" s="66"/>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A78" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B78" s="31"/>
+      <c r="C78" s="31"/>
+      <c r="D78" s="32"/>
+      <c r="E78" s="32"/>
+      <c r="F78" s="32"/>
+      <c r="G78" s="44"/>
+      <c r="H78" s="67" t="s">
+        <v>58</v>
+      </c>
+      <c r="I78" s="67"/>
+      <c r="J78" s="67"/>
+      <c r="K78" s="68"/>
+      <c r="L78" s="67"/>
+      <c r="M78" s="67"/>
+      <c r="N78" s="69"/>
+    </row>
+    <row r="79" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="B79" s="36"/>
+      <c r="C79" s="36"/>
+      <c r="D79" s="36"/>
+      <c r="E79" s="36"/>
+      <c r="F79" s="36"/>
+      <c r="G79" s="37"/>
+      <c r="H79" s="70"/>
+      <c r="I79" s="71"/>
+      <c r="J79" s="71"/>
+      <c r="K79" s="71"/>
+      <c r="L79" s="71"/>
+      <c r="M79" s="71"/>
+      <c r="N79" s="72"/>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C80" s="38"/>
+      <c r="D80" s="38"/>
+      <c r="E80" s="38"/>
+      <c r="F80" s="38"/>
+      <c r="G80" s="38"/>
+    </row>
+    <row r="81" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A82" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="L65" s="63"/>
-      <c r="M65" s="63"/>
-      <c r="N65" s="66"/>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A66" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="B66" s="31"/>
-      <c r="C66" s="31"/>
-      <c r="D66" s="32"/>
-      <c r="E66" s="32"/>
-      <c r="F66" s="32"/>
-      <c r="G66" s="44"/>
-      <c r="H66" s="67" t="s">
-        <v>19</v>
-      </c>
-      <c r="I66" s="67"/>
-      <c r="J66" s="67"/>
-      <c r="K66" s="68">
-        <v>24</v>
-      </c>
-      <c r="L66" s="67"/>
-      <c r="M66" s="67"/>
-      <c r="N66" s="69"/>
-    </row>
-    <row r="67" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="B67" s="36"/>
-      <c r="C67" s="36"/>
-      <c r="D67" s="36"/>
-      <c r="E67" s="36"/>
-      <c r="F67" s="36"/>
-      <c r="G67" s="37"/>
-      <c r="H67" s="70"/>
-      <c r="I67" s="71"/>
-      <c r="J67" s="71"/>
-      <c r="K67" s="71"/>
-      <c r="L67" s="71"/>
-      <c r="M67" s="71"/>
-      <c r="N67" s="72"/>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C68" s="38"/>
-      <c r="D68" s="38"/>
-      <c r="E68" s="38"/>
-      <c r="F68" s="38"/>
-      <c r="G68" s="38"/>
-    </row>
-    <row r="69" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A70" s="73" t="s">
-        <v>24</v>
-      </c>
-      <c r="B70" s="74"/>
-      <c r="C70" s="74"/>
-      <c r="D70" s="74"/>
-      <c r="E70" s="75" t="s">
+      <c r="B82" s="74"/>
+      <c r="C82" s="74"/>
+      <c r="D82" s="74"/>
+      <c r="E82" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="F70" s="76"/>
-      <c r="G70" s="75" t="s">
+      <c r="F82" s="76"/>
+      <c r="G82" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="H70" s="76"/>
-      <c r="I70" s="74" t="s">
+      <c r="H82" s="76"/>
+      <c r="I82" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="J70" s="74"/>
-      <c r="K70" s="74" t="s">
+      <c r="J82" s="74"/>
+      <c r="K82" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="L70" s="74"/>
-      <c r="M70" s="74" t="s">
+      <c r="L82" s="74"/>
+      <c r="M82" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="N70" s="83"/>
-      <c r="O70" s="39"/>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A71" s="86" t="s">
+      <c r="N82" s="83"/>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A83" s="86" t="s">
         <v>30</v>
       </c>
-      <c r="B71" s="81"/>
-      <c r="C71" s="94" t="s">
+      <c r="B83" s="81"/>
+      <c r="C83" s="94" t="s">
         <v>31</v>
       </c>
-      <c r="D71" s="94"/>
-      <c r="E71" s="77"/>
-      <c r="F71" s="78"/>
-      <c r="G71" s="77"/>
-      <c r="H71" s="78"/>
-      <c r="I71" s="81"/>
-      <c r="J71" s="81"/>
-      <c r="K71" s="81"/>
-      <c r="L71" s="81"/>
-      <c r="M71" s="81"/>
-      <c r="N71" s="84"/>
-      <c r="O71" s="39"/>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A72" s="86"/>
-      <c r="B72" s="81"/>
-      <c r="C72" s="94"/>
-      <c r="D72" s="94"/>
-      <c r="E72" s="77"/>
-      <c r="F72" s="78"/>
-      <c r="G72" s="77"/>
-      <c r="H72" s="78"/>
-      <c r="I72" s="81"/>
-      <c r="J72" s="81"/>
-      <c r="K72" s="81"/>
-      <c r="L72" s="81"/>
-      <c r="M72" s="81"/>
-      <c r="N72" s="84"/>
-      <c r="O72" s="39"/>
-    </row>
-    <row r="73" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="87"/>
-      <c r="B73" s="82"/>
-      <c r="C73" s="95"/>
-      <c r="D73" s="95"/>
-      <c r="E73" s="79"/>
-      <c r="F73" s="80"/>
-      <c r="G73" s="79"/>
-      <c r="H73" s="80"/>
-      <c r="I73" s="82"/>
-      <c r="J73" s="82"/>
-      <c r="K73" s="82"/>
-      <c r="L73" s="82"/>
-      <c r="M73" s="82"/>
-      <c r="N73" s="85"/>
-      <c r="O73" s="39"/>
-    </row>
-    <row r="74" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="55">
-        <v>100</v>
-      </c>
-      <c r="B74" s="56"/>
-      <c r="C74" s="57"/>
-      <c r="D74" s="57"/>
-      <c r="E74" s="58"/>
-      <c r="F74" s="59"/>
-      <c r="G74" s="58"/>
-      <c r="H74" s="59"/>
-      <c r="I74" s="60"/>
-      <c r="J74" s="60"/>
-      <c r="K74" s="60"/>
-      <c r="L74" s="60"/>
-      <c r="M74" s="61"/>
-      <c r="N74" s="62"/>
-    </row>
-    <row r="76" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="B76" s="12"/>
-      <c r="C76" s="6"/>
-      <c r="D76" s="6"/>
-      <c r="E76" s="6"/>
-      <c r="F76" s="6"/>
-      <c r="G76" s="6"/>
-      <c r="H76" s="6"/>
-      <c r="I76" s="6"/>
-      <c r="J76" s="6"/>
-      <c r="K76" s="6"/>
-      <c r="L76" s="6"/>
-      <c r="M76" s="6"/>
-      <c r="N76" s="6"/>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A77" s="88"/>
-      <c r="B77" s="89"/>
-      <c r="C77" s="89"/>
-      <c r="D77" s="89"/>
-      <c r="E77" s="89"/>
-      <c r="F77" s="89"/>
-      <c r="G77" s="90"/>
-      <c r="H77" s="89" t="s">
-        <v>14</v>
-      </c>
-      <c r="I77" s="89"/>
-      <c r="J77" s="89"/>
-      <c r="K77" s="137" t="s">
-        <v>15</v>
-      </c>
-      <c r="L77" s="138"/>
-      <c r="M77" s="138"/>
-      <c r="N77" s="139"/>
-    </row>
-    <row r="78" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="91"/>
-      <c r="B78" s="92"/>
-      <c r="C78" s="92"/>
-      <c r="D78" s="92"/>
-      <c r="E78" s="92"/>
-      <c r="F78" s="92"/>
-      <c r="G78" s="93"/>
-      <c r="H78" s="92"/>
-      <c r="I78" s="92"/>
-      <c r="J78" s="92"/>
-      <c r="K78" s="97" t="s">
-        <v>16</v>
-      </c>
-      <c r="L78" s="140"/>
-      <c r="M78" s="97" t="s">
-        <v>17</v>
-      </c>
-      <c r="N78" s="93"/>
-    </row>
-    <row r="79" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="B79" s="27"/>
-      <c r="C79" s="27"/>
-      <c r="D79" s="28"/>
-      <c r="E79" s="28"/>
-      <c r="F79" s="28"/>
-      <c r="G79" s="29"/>
-      <c r="H79" s="63"/>
-      <c r="I79" s="63"/>
-      <c r="J79" s="63"/>
-      <c r="K79" s="64"/>
-      <c r="L79" s="65"/>
-      <c r="M79" s="64"/>
-      <c r="N79" s="66"/>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A80" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="B80" s="31"/>
-      <c r="C80" s="31"/>
-      <c r="D80" s="32"/>
-      <c r="E80" s="32"/>
-      <c r="F80" s="32"/>
-      <c r="G80" s="44"/>
-      <c r="H80" s="67" t="s">
-        <v>46</v>
-      </c>
-      <c r="I80" s="67"/>
-      <c r="J80" s="67"/>
-      <c r="K80" s="68"/>
-      <c r="L80" s="67"/>
-      <c r="M80" s="68"/>
-      <c r="N80" s="69"/>
-    </row>
-    <row r="81" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="B81" s="36"/>
-      <c r="C81" s="36"/>
-      <c r="D81" s="36"/>
-      <c r="E81" s="36"/>
-      <c r="F81" s="36"/>
-      <c r="G81" s="37"/>
-      <c r="H81" s="70"/>
-      <c r="I81" s="71"/>
-      <c r="J81" s="71"/>
-      <c r="K81" s="71"/>
-      <c r="L81" s="71"/>
-      <c r="M81" s="71"/>
-      <c r="N81" s="72"/>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C82" s="38"/>
-      <c r="D82" s="38"/>
-      <c r="E82" s="38"/>
-      <c r="F82" s="38"/>
-      <c r="G82" s="38"/>
-    </row>
-    <row r="83" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="D83" s="94"/>
+      <c r="E83" s="77"/>
+      <c r="F83" s="78"/>
+      <c r="G83" s="77"/>
+      <c r="H83" s="78"/>
+      <c r="I83" s="81"/>
+      <c r="J83" s="81"/>
+      <c r="K83" s="81"/>
+      <c r="L83" s="81"/>
+      <c r="M83" s="81"/>
+      <c r="N83" s="84"/>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A84" s="73" t="s">
-        <v>24</v>
-      </c>
-      <c r="B84" s="74"/>
-      <c r="C84" s="74"/>
-      <c r="D84" s="74"/>
-      <c r="E84" s="75" t="s">
+      <c r="A84" s="86"/>
+      <c r="B84" s="81"/>
+      <c r="C84" s="94"/>
+      <c r="D84" s="94"/>
+      <c r="E84" s="77"/>
+      <c r="F84" s="78"/>
+      <c r="G84" s="77"/>
+      <c r="H84" s="78"/>
+      <c r="I84" s="81"/>
+      <c r="J84" s="81"/>
+      <c r="K84" s="81"/>
+      <c r="L84" s="81"/>
+      <c r="M84" s="81"/>
+      <c r="N84" s="84"/>
+    </row>
+    <row r="85" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="87"/>
+      <c r="B85" s="82"/>
+      <c r="C85" s="95"/>
+      <c r="D85" s="95"/>
+      <c r="E85" s="79"/>
+      <c r="F85" s="80"/>
+      <c r="G85" s="79"/>
+      <c r="H85" s="80"/>
+      <c r="I85" s="82"/>
+      <c r="J85" s="82"/>
+      <c r="K85" s="82"/>
+      <c r="L85" s="82"/>
+      <c r="M85" s="82"/>
+      <c r="N85" s="85"/>
+    </row>
+    <row r="86" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A86" s="98">
+        <v>5</v>
+      </c>
+      <c r="B86" s="99"/>
+      <c r="C86" s="100"/>
+      <c r="D86" s="100"/>
+      <c r="E86" s="101"/>
+      <c r="F86" s="102"/>
+      <c r="G86" s="101"/>
+      <c r="H86" s="102"/>
+      <c r="I86" s="103"/>
+      <c r="J86" s="103"/>
+      <c r="K86" s="103"/>
+      <c r="L86" s="103"/>
+      <c r="M86" s="104"/>
+      <c r="N86" s="105"/>
+    </row>
+    <row r="87" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A87" s="98">
         <v>25</v>
       </c>
-      <c r="F84" s="76"/>
-      <c r="G84" s="75" t="s">
-        <v>26</v>
-      </c>
-      <c r="H84" s="76"/>
-      <c r="I84" s="74" t="s">
-        <v>27</v>
-      </c>
-      <c r="J84" s="74"/>
-      <c r="K84" s="74" t="s">
-        <v>28</v>
-      </c>
-      <c r="L84" s="74"/>
-      <c r="M84" s="74" t="s">
-        <v>29</v>
-      </c>
-      <c r="N84" s="83"/>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A85" s="86" t="s">
-        <v>30</v>
-      </c>
-      <c r="B85" s="81"/>
-      <c r="C85" s="94" t="s">
-        <v>31</v>
-      </c>
-      <c r="D85" s="94"/>
-      <c r="E85" s="77"/>
-      <c r="F85" s="78"/>
-      <c r="G85" s="77"/>
-      <c r="H85" s="78"/>
-      <c r="I85" s="81"/>
-      <c r="J85" s="81"/>
-      <c r="K85" s="81"/>
-      <c r="L85" s="81"/>
-      <c r="M85" s="81"/>
-      <c r="N85" s="84"/>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A86" s="86"/>
-      <c r="B86" s="81"/>
-      <c r="C86" s="94"/>
-      <c r="D86" s="94"/>
-      <c r="E86" s="77"/>
-      <c r="F86" s="78"/>
-      <c r="G86" s="77"/>
-      <c r="H86" s="78"/>
-      <c r="I86" s="81"/>
-      <c r="J86" s="81"/>
-      <c r="K86" s="81"/>
-      <c r="L86" s="81"/>
-      <c r="M86" s="81"/>
-      <c r="N86" s="84"/>
-    </row>
-    <row r="87" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="87"/>
-      <c r="B87" s="82"/>
-      <c r="C87" s="95"/>
-      <c r="D87" s="95"/>
-      <c r="E87" s="79"/>
-      <c r="F87" s="80"/>
-      <c r="G87" s="79"/>
-      <c r="H87" s="80"/>
-      <c r="I87" s="82"/>
-      <c r="J87" s="82"/>
-      <c r="K87" s="82"/>
-      <c r="L87" s="82"/>
-      <c r="M87" s="82"/>
-      <c r="N87" s="85"/>
+      <c r="B87" s="99"/>
+      <c r="C87" s="100"/>
+      <c r="D87" s="100"/>
+      <c r="E87" s="101"/>
+      <c r="F87" s="102"/>
+      <c r="G87" s="101"/>
+      <c r="H87" s="102"/>
+      <c r="I87" s="103"/>
+      <c r="J87" s="103"/>
+      <c r="K87" s="103"/>
+      <c r="L87" s="103"/>
+      <c r="M87" s="104"/>
+      <c r="N87" s="105"/>
     </row>
     <row r="88" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="98">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B88" s="99"/>
       <c r="C88" s="100"/>
@@ -3033,7 +3032,7 @@
     </row>
     <row r="89" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="98">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="B89" s="99"/>
       <c r="C89" s="100"/>
@@ -3049,139 +3048,89 @@
       <c r="M89" s="104"/>
       <c r="N89" s="105"/>
     </row>
-    <row r="90" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A90" s="98">
-        <v>50</v>
-      </c>
-      <c r="B90" s="99"/>
-      <c r="C90" s="100"/>
-      <c r="D90" s="100"/>
-      <c r="E90" s="101"/>
-      <c r="F90" s="102"/>
-      <c r="G90" s="101"/>
-      <c r="H90" s="102"/>
-      <c r="I90" s="103"/>
-      <c r="J90" s="103"/>
-      <c r="K90" s="103"/>
-      <c r="L90" s="103"/>
-      <c r="M90" s="104"/>
-      <c r="N90" s="105"/>
+    <row r="90" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="55">
+        <v>95</v>
+      </c>
+      <c r="B90" s="56"/>
+      <c r="C90" s="57"/>
+      <c r="D90" s="57"/>
+      <c r="E90" s="58"/>
+      <c r="F90" s="59"/>
+      <c r="G90" s="58"/>
+      <c r="H90" s="59"/>
+      <c r="I90" s="60"/>
+      <c r="J90" s="60"/>
+      <c r="K90" s="60"/>
+      <c r="L90" s="60"/>
+      <c r="M90" s="61"/>
+      <c r="N90" s="62"/>
     </row>
     <row r="91" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A91" s="98">
-        <v>75</v>
-      </c>
-      <c r="B91" s="99"/>
-      <c r="C91" s="100"/>
-      <c r="D91" s="100"/>
-      <c r="E91" s="101"/>
-      <c r="F91" s="102"/>
-      <c r="G91" s="101"/>
-      <c r="H91" s="102"/>
-      <c r="I91" s="103"/>
-      <c r="J91" s="103"/>
-      <c r="K91" s="103"/>
-      <c r="L91" s="103"/>
-      <c r="M91" s="104"/>
-      <c r="N91" s="105"/>
-    </row>
-    <row r="92" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="55">
-        <v>95</v>
-      </c>
-      <c r="B92" s="56"/>
-      <c r="C92" s="57"/>
-      <c r="D92" s="57"/>
-      <c r="E92" s="58"/>
-      <c r="F92" s="59"/>
-      <c r="G92" s="58"/>
-      <c r="H92" s="59"/>
-      <c r="I92" s="60"/>
-      <c r="J92" s="60"/>
-      <c r="K92" s="60"/>
-      <c r="L92" s="60"/>
-      <c r="M92" s="61"/>
-      <c r="N92" s="62"/>
-    </row>
-    <row r="93" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A93" s="3"/>
-      <c r="B93" s="3"/>
-      <c r="C93" s="47"/>
-      <c r="D93" s="47"/>
-      <c r="E93" s="48"/>
-      <c r="F93" s="48"/>
-      <c r="G93" s="48"/>
-      <c r="H93" s="48"/>
-      <c r="I93" s="48"/>
-      <c r="J93" s="48"/>
-      <c r="K93" s="48"/>
-      <c r="L93" s="48"/>
-      <c r="M93" s="49"/>
-      <c r="N93" s="49"/>
-    </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B95" s="40" t="s">
+      <c r="A91" s="3"/>
+      <c r="B91" s="3"/>
+      <c r="C91" s="47"/>
+      <c r="D91" s="47"/>
+      <c r="E91" s="48"/>
+      <c r="F91" s="48"/>
+      <c r="G91" s="48"/>
+      <c r="H91" s="48"/>
+      <c r="I91" s="48"/>
+      <c r="J91" s="48"/>
+      <c r="K91" s="48"/>
+      <c r="L91" s="48"/>
+      <c r="M91" s="49"/>
+      <c r="N91" s="49"/>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B93" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C93" s="40"/>
+      <c r="D93" s="40"/>
+      <c r="E93" s="40"/>
+      <c r="F93" s="40"/>
+      <c r="G93" s="40"/>
+      <c r="H93" s="40"/>
+      <c r="I93" s="40"/>
+    </row>
+    <row r="94" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="95" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="C95" s="40"/>
-      <c r="D95" s="40"/>
-      <c r="E95" s="40"/>
-      <c r="F95" s="40"/>
-      <c r="G95" s="40"/>
-      <c r="H95" s="40"/>
-      <c r="I95" s="40"/>
-    </row>
-    <row r="96" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="97" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="50" t="s">
+      <c r="B95" s="50"/>
+      <c r="C95" s="50"/>
+      <c r="D95" s="50"/>
+      <c r="E95" s="50"/>
+      <c r="F95" s="50"/>
+      <c r="G95" s="51"/>
+      <c r="H95" s="52"/>
+      <c r="I95" s="52"/>
+      <c r="J95" s="52"/>
+      <c r="K95" s="52"/>
+      <c r="L95" s="52"/>
+      <c r="M95" s="52"/>
+      <c r="N95" s="53"/>
+    </row>
+    <row r="97" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B97" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="B97" s="50"/>
-      <c r="C97" s="50"/>
-      <c r="D97" s="50"/>
-      <c r="E97" s="50"/>
-      <c r="F97" s="50"/>
-      <c r="G97" s="51"/>
-      <c r="H97" s="52"/>
-      <c r="I97" s="52"/>
-      <c r="J97" s="52"/>
-      <c r="K97" s="52"/>
-      <c r="L97" s="52"/>
-      <c r="M97" s="52"/>
-      <c r="N97" s="53"/>
-    </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B99" s="41" t="s">
+      <c r="C97" s="42"/>
+      <c r="D97" s="42"/>
+      <c r="E97" s="42"/>
+      <c r="I97" s="54"/>
+      <c r="J97" s="54"/>
+      <c r="K97" s="54"/>
+    </row>
+    <row r="98" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="D98" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="C99" s="42"/>
-      <c r="D99" s="42"/>
-      <c r="E99" s="42"/>
-      <c r="I99" s="54"/>
-      <c r="J99" s="54"/>
-      <c r="K99" s="54"/>
-    </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D100" s="43" t="s">
-        <v>36</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="168">
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="E91:F91"/>
-    <mergeCell ref="G91:H91"/>
-    <mergeCell ref="I91:J91"/>
-    <mergeCell ref="K91:L91"/>
-    <mergeCell ref="M91:N91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="E92:F92"/>
-    <mergeCell ref="G92:H92"/>
-    <mergeCell ref="I92:J92"/>
-    <mergeCell ref="K92:L92"/>
-    <mergeCell ref="M92:N92"/>
+  <mergeCells count="163">
     <mergeCell ref="A89:B89"/>
     <mergeCell ref="C89:D89"/>
     <mergeCell ref="E89:F89"/>
@@ -3196,15 +3145,30 @@
     <mergeCell ref="I90:J90"/>
     <mergeCell ref="K90:L90"/>
     <mergeCell ref="M90:N90"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="E87:F87"/>
+    <mergeCell ref="G87:H87"/>
+    <mergeCell ref="I87:J87"/>
+    <mergeCell ref="K87:L87"/>
+    <mergeCell ref="M87:N87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="E88:F88"/>
+    <mergeCell ref="G88:H88"/>
+    <mergeCell ref="I88:J88"/>
+    <mergeCell ref="K88:L88"/>
+    <mergeCell ref="M88:N88"/>
     <mergeCell ref="M31:N31"/>
-    <mergeCell ref="A84:D84"/>
-    <mergeCell ref="E84:F87"/>
-    <mergeCell ref="G84:H87"/>
-    <mergeCell ref="I84:J87"/>
-    <mergeCell ref="K84:L87"/>
-    <mergeCell ref="M84:N87"/>
-    <mergeCell ref="A85:B87"/>
-    <mergeCell ref="C85:D87"/>
+    <mergeCell ref="A82:D82"/>
+    <mergeCell ref="E82:F85"/>
+    <mergeCell ref="G82:H85"/>
+    <mergeCell ref="I82:J85"/>
+    <mergeCell ref="K82:L85"/>
+    <mergeCell ref="M82:N85"/>
+    <mergeCell ref="A83:B85"/>
+    <mergeCell ref="C83:D85"/>
+    <mergeCell ref="K78:N78"/>
     <mergeCell ref="H34:N34"/>
     <mergeCell ref="B1:M1"/>
     <mergeCell ref="B20:M20"/>
@@ -3212,11 +3176,11 @@
     <mergeCell ref="G22:N23"/>
     <mergeCell ref="A24:F25"/>
     <mergeCell ref="G24:N25"/>
-    <mergeCell ref="A77:G78"/>
-    <mergeCell ref="H77:J78"/>
-    <mergeCell ref="K77:N77"/>
-    <mergeCell ref="K78:L78"/>
-    <mergeCell ref="M78:N78"/>
+    <mergeCell ref="A75:G76"/>
+    <mergeCell ref="H75:J76"/>
+    <mergeCell ref="K75:N75"/>
+    <mergeCell ref="K76:L76"/>
+    <mergeCell ref="M76:N76"/>
     <mergeCell ref="H32:J32"/>
     <mergeCell ref="K32:L32"/>
     <mergeCell ref="M32:N32"/>
@@ -3267,7 +3231,6 @@
     <mergeCell ref="I44:J44"/>
     <mergeCell ref="K44:L44"/>
     <mergeCell ref="H51:J51"/>
-    <mergeCell ref="H52:J52"/>
     <mergeCell ref="M46:N46"/>
     <mergeCell ref="A49:G50"/>
     <mergeCell ref="H49:J50"/>
@@ -3278,64 +3241,59 @@
     <mergeCell ref="I46:J46"/>
     <mergeCell ref="K46:L46"/>
     <mergeCell ref="K51:N51"/>
-    <mergeCell ref="K52:N52"/>
     <mergeCell ref="K49:N50"/>
-    <mergeCell ref="C57:D59"/>
-    <mergeCell ref="H53:N53"/>
-    <mergeCell ref="A56:D56"/>
-    <mergeCell ref="E56:F59"/>
-    <mergeCell ref="G56:H59"/>
-    <mergeCell ref="I56:J59"/>
-    <mergeCell ref="K56:L59"/>
-    <mergeCell ref="M56:N59"/>
-    <mergeCell ref="A57:B59"/>
-    <mergeCell ref="A63:G64"/>
-    <mergeCell ref="H63:J64"/>
-    <mergeCell ref="C71:D73"/>
-    <mergeCell ref="K63:N64"/>
-    <mergeCell ref="K66:N66"/>
-    <mergeCell ref="K65:N65"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="E60:F60"/>
-    <mergeCell ref="G60:H60"/>
-    <mergeCell ref="I60:J60"/>
-    <mergeCell ref="K60:L60"/>
-    <mergeCell ref="M60:N60"/>
-    <mergeCell ref="H65:J65"/>
-    <mergeCell ref="H67:N67"/>
-    <mergeCell ref="A70:D70"/>
-    <mergeCell ref="E70:F73"/>
-    <mergeCell ref="G70:H73"/>
-    <mergeCell ref="I70:J73"/>
-    <mergeCell ref="K70:L73"/>
-    <mergeCell ref="M70:N73"/>
-    <mergeCell ref="A71:B73"/>
-    <mergeCell ref="H66:J66"/>
-    <mergeCell ref="A97:F97"/>
-    <mergeCell ref="G97:N97"/>
-    <mergeCell ref="I99:K99"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="E74:F74"/>
-    <mergeCell ref="G74:H74"/>
-    <mergeCell ref="I74:J74"/>
-    <mergeCell ref="K74:L74"/>
-    <mergeCell ref="M74:N74"/>
-    <mergeCell ref="H79:J79"/>
-    <mergeCell ref="K79:L79"/>
-    <mergeCell ref="M79:N79"/>
-    <mergeCell ref="H80:J80"/>
-    <mergeCell ref="K80:L80"/>
-    <mergeCell ref="M80:N80"/>
-    <mergeCell ref="H81:N81"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="E88:F88"/>
-    <mergeCell ref="G88:H88"/>
-    <mergeCell ref="I88:J88"/>
-    <mergeCell ref="K88:L88"/>
-    <mergeCell ref="M88:N88"/>
+    <mergeCell ref="C56:D58"/>
+    <mergeCell ref="H52:N52"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="E55:F58"/>
+    <mergeCell ref="G55:H58"/>
+    <mergeCell ref="I55:J58"/>
+    <mergeCell ref="K55:L58"/>
+    <mergeCell ref="M55:N58"/>
+    <mergeCell ref="A56:B58"/>
+    <mergeCell ref="A62:G63"/>
+    <mergeCell ref="H62:J63"/>
+    <mergeCell ref="C69:D71"/>
+    <mergeCell ref="K62:N63"/>
+    <mergeCell ref="K64:N64"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="G59:H59"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="K59:L59"/>
+    <mergeCell ref="M59:N59"/>
+    <mergeCell ref="H65:N65"/>
+    <mergeCell ref="A68:D68"/>
+    <mergeCell ref="E68:F71"/>
+    <mergeCell ref="G68:H71"/>
+    <mergeCell ref="I68:J71"/>
+    <mergeCell ref="K68:L71"/>
+    <mergeCell ref="M68:N71"/>
+    <mergeCell ref="A69:B71"/>
+    <mergeCell ref="H64:J64"/>
+    <mergeCell ref="A95:F95"/>
+    <mergeCell ref="G95:N95"/>
+    <mergeCell ref="I97:K97"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="E72:F72"/>
+    <mergeCell ref="G72:H72"/>
+    <mergeCell ref="I72:J72"/>
+    <mergeCell ref="K72:L72"/>
+    <mergeCell ref="M72:N72"/>
+    <mergeCell ref="H77:J77"/>
+    <mergeCell ref="K77:L77"/>
+    <mergeCell ref="M77:N77"/>
+    <mergeCell ref="H78:J78"/>
+    <mergeCell ref="H79:N79"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="E86:F86"/>
+    <mergeCell ref="G86:H86"/>
+    <mergeCell ref="I86:J86"/>
+    <mergeCell ref="K86:L86"/>
+    <mergeCell ref="M86:N86"/>
   </mergeCells>
   <pageMargins left="0.59055118110236227" right="0.19685039370078741" top="0.59055118110236227" bottom="0.19685039370078741" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>